<commit_message>
1. Making number of episodes     a scale up factor in discrete tests 2.  Changing world3 continuous to have a reward of '1'.
</commit_message>
<xml_diff>
--- a/results/WorldUnknown/MeansAndSTDDisc.xlsx
+++ b/results/WorldUnknown/MeansAndSTDDisc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luker\source\repos\ReinforcementLearning\results\WorldUnknown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA257F2-DD6E-4F2A-BC29-54C077921D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FC72C9-1F75-44C3-B58D-5EA4D5EA1936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
     <t>SARSA0.75 - Mean</t>
   </si>
   <si>
-    <t>SARSA0.75 - STD</t>
+    <t>numEpisodes</t>
   </si>
 </sst>
 </file>
@@ -376,7 +376,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -386,13 +386,13 @@
     <col min="3" max="3" width="12.89453125" customWidth="1"/>
     <col min="4" max="4" width="12.05078125" customWidth="1"/>
     <col min="5" max="5" width="11.9453125" customWidth="1"/>
-    <col min="6" max="6" width="11.26171875" customWidth="1"/>
-    <col min="7" max="7" width="15.41796875" customWidth="1"/>
-    <col min="8" max="8" width="13.7890625" customWidth="1"/>
+    <col min="6" max="6" width="12.15625" customWidth="1"/>
+    <col min="7" max="7" width="10.62890625" customWidth="1"/>
+    <col min="8" max="8" width="15.578125" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="10" max="10" width="14.3125" customWidth="1"/>
-    <col min="11" max="11" width="15.578125" customWidth="1"/>
-    <col min="12" max="12" width="14.41796875" customWidth="1"/>
+    <col min="11" max="11" width="13.68359375" customWidth="1"/>
+    <col min="12" max="12" width="15.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -409,28 +409,28 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing orientatino of the heatmap to be more accurate
</commit_message>
<xml_diff>
--- a/results/WorldUnknown/MeansAndSTDDisc.xlsx
+++ b/results/WorldUnknown/MeansAndSTDDisc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luker\source\repos\ReinforcementLearning\results\WorldUnknown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FC72C9-1F75-44C3-B58D-5EA4D5EA1936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454AA37D-67A5-4B80-9260-8338362BE903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,6 +34,9 @@
     <t>maxNumTries</t>
   </si>
   <si>
+    <t>numEpisodes</t>
+  </si>
+  <si>
     <t>Qlearn - Mean</t>
   </si>
   <si>
@@ -53,9 +56,6 @@
   </si>
   <si>
     <t>SARSA0.75 - Mean</t>
-  </si>
-  <si>
-    <t>numEpisodes</t>
   </si>
 </sst>
 </file>
@@ -376,7 +376,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="M15" sqref="A2:M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -409,28 +409,28 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>